<commit_message>
Working on database Generation
</commit_message>
<xml_diff>
--- a/Ground Seg/scripts/BeaconDefinition.xlsx
+++ b/Ground Seg/scripts/BeaconDefinition.xlsx
@@ -79,6 +79,7 @@
   <fonts count="2">
     <font>
       <i val="0"/>
+      <color rgb="FF000000"/>
       <name val="Sans"/>
       <strike val="0"/>
     </font>
@@ -91,19 +92,19 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill/>
+    </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
+    <border>
       <right style="none">
         <color rgb="FFC7C7C7"/>
       </right>
@@ -124,10 +125,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -142,13 +143,21 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView topLeftCell="A16" workbookViewId="0" tabSelected="1">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="9" style="1" width="9.142308"/>
+    <col min="1" max="1" style="1" width="25.56989" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="1" width="37.71202" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" style="1" width="12.14213" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="1" width="10.71364" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" style="1" width="10.99934" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" style="1" width="12.85637" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" style="1" width="10.71364" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="1" width="24.4271" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="9.142308"/>
     <col min="10" max="16384" style="1"/>
   </cols>
   <sheetData>
@@ -195,10 +204,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -1355,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F42">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
         <v>2</v>
@@ -1367,123 +1376,6 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" t="s">
-        <v>3</v>
-      </c>
-      <c r="I45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" t="str">
-        <v>Total Bytes:</v>
-      </c>
-      <c r="F46">
-        <f>SUM(F2:F42)</f>
-        <v>146</v>
-      </c>
-      <c r="G46" t="s">
-        <v>3</v>
-      </c>
-      <c r="H46" t="s">
-        <v>3</v>
-      </c>
-      <c r="I46" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified generalReader.py to use the length of the file instead of user input.
Changed the telemetry definition as well for easier use
</commit_message>
<xml_diff>
--- a/Ground Seg/scripts/BeaconDefinition.xlsx
+++ b/Ground Seg/scripts/BeaconDefinition.xlsx
@@ -100,13 +100,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="0" diagonalDown="0">
+    <border diagonalDown="0">
       <left style="none">
         <color rgb="FFC7C7C7"/>
       </left>
-      <right style="none">
+      <bottom style="none">
         <color rgb="FFC7C7C7"/>
-      </right>
+      </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
       <left style="none">
@@ -142,13 +142,21 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView topLeftCell="A21" workbookViewId="0" tabSelected="1">
+      <selection activeCell="I46" sqref="A43:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="9" style="1" width="9.142308"/>
+    <col min="1" max="1" style="1" width="25.56989" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="1" width="37.71202" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" style="1" width="12.14213" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="1" width="9.142308"/>
+    <col min="5" max="5" style="1" width="10.99934" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" style="1" width="12.85637" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" style="1" width="10.71364" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="1" width="24.4271" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="9.142308"/>
     <col min="10" max="16384" style="1"/>
   </cols>
   <sheetData>
@@ -1367,123 +1375,6 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" t="s">
-        <v>3</v>
-      </c>
-      <c r="I45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" t="str">
-        <v>Total Bytes:</v>
-      </c>
-      <c r="F46">
-        <f>SUM(F2:F42)</f>
-        <v>146</v>
-      </c>
-      <c r="G46" t="s">
-        <v>3</v>
-      </c>
-      <c r="H46" t="s">
-        <v>3</v>
-      </c>
-      <c r="I46" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>